<commit_message>
toeuserauth tables added, actions added
</commit_message>
<xml_diff>
--- a/contracts_table.xlsx
+++ b/contracts_table.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding\github_repos\toe_contracts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E934A36A-ED7C-492A-8BE9-8ACE79D5C8CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="auth" sheetId="5" r:id="rId1"/>
@@ -14,22 +20,16 @@
     <sheet name="ridex" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
   <si>
     <t>ram_payer</t>
   </si>
@@ -177,12 +177,98 @@
   <si>
     <t>online</t>
   </si>
+  <si>
+    <t>toe1userauth</t>
+  </si>
+  <si>
+    <t>user.value</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>user i..e user.value</t>
+  </si>
+  <si>
+    <t>$ cleost get table toe1userauth toedri111111 users</t>
+  </si>
+  <si>
+    <t>$ cleost get table toe1userauth toedri111111 users
+{
+  "rows": [{
+      "user": "toedri111111",
+      "type": "driver",
+      "profile_hash": "e5deda7cafa7b8c861b352e34d6741461ee17a7c2385a0f86763e9ab3298c385",
+      "user_status": "added",
+      "add_timestamp": 1596366825,
+      "update_timestamp": 0,
+      "verify_timestamp": 0,
+      "blist_timestamp": 0,
+      "validator_verify": "",
+      "validator_blacklist": "",
+      "rating": "0.00000000000000000",
+      "ride_total": 0,
+      "ride_rated": 0
+    }
+  ],
+  "more": false,
+  "next_key": ""
+}</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>profile_hash</t>
+  </si>
+  <si>
+    <t>user_status</t>
+  </si>
+  <si>
+    <t>add_timestamp</t>
+  </si>
+  <si>
+    <t>update_timestamp</t>
+  </si>
+  <si>
+    <t>verify_timestamp</t>
+  </si>
+  <si>
+    <t>blist_timestamp</t>
+  </si>
+  <si>
+    <t>validator_verify</t>
+  </si>
+  <si>
+    <t>validator_blacklist</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>ride_total</t>
+  </si>
+  <si>
+    <t>ride_rated</t>
+  </si>
+  <si>
+    <t>toedri111111</t>
+  </si>
+  <si>
+    <t>driver</t>
+  </si>
+  <si>
+    <t>e5deda7cafa7b8c861b352e34d6741461ee17a7c2385a0f86763e9ab3298c385</t>
+  </si>
+  <si>
+    <t>added</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -405,14 +491,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,124 +808,343 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="H1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="H2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="5">
+        <v>1596366825</v>
+      </c>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5">
+        <v>0</v>
+      </c>
+      <c r="S2" s="5">
+        <v>0</v>
+      </c>
+      <c r="T2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:F17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="A24" sqref="A24:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1"/>
-    <row r="9" spans="1:6">
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D9" s="7" t="s">
         <v>10</v>
       </c>
@@ -847,7 +1155,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
@@ -858,178 +1166,178 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1">
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1">
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G21" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1">
+    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G22" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="D24" s="15"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1">
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+    </row>
+    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G31" s="7" t="s">
         <v>33</v>
       </c>
@@ -1037,7 +1345,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1">
+    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G32" s="4">
         <v>2020</v>
       </c>
@@ -1057,107 +1365,107 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A21:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="D21" s="15"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1">
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+    </row>
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G28" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="H28" s="15"/>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H28" s="13"/>
+    </row>
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G29" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="H29" s="16"/>
+      <c r="H29" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1168,24 +1476,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>